<commit_message>
New species, fresh and albatross data
New species A. endrachtensis, fresh lwr data and figures, and matching data and figures from Albatross collection for comparison.
</commit_message>
<xml_diff>
--- a/Albatross_Raw_Data/Albatross_LWR_Raw_Data.xlsx
+++ b/Albatross_Raw_Data/Albatross_LWR_Raw_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabes\Documents\AlbatrossPhillipinesLWR\Albatross_Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D084F3-A976-4692-B594-0A7617B68A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768CCE9-984C-43B1-B549-47BF45248FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="39">
   <si>
     <t>Species</t>
   </si>
@@ -145,6 +145,12 @@
   <si>
     <t>Doboatherina_duodecimalis</t>
   </si>
+  <si>
+    <t>Atherinomorus_endrachtensis</t>
+  </si>
+  <si>
+    <t>7_17_2023</t>
+  </si>
 </sst>
 </file>
 
@@ -162,12 +168,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -178,6 +186,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -424,11 +433,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K747"/>
+  <dimension ref="A1:K879"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A550" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A623" sqref="A623"/>
+      <pane ySplit="1" topLeftCell="A727" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F872" sqref="F872"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -23002,7 +23011,7 @@
         <v>4.5</v>
       </c>
       <c r="H664" s="2">
-        <f t="shared" ref="H664:H747" si="473">F664/10</f>
+        <f t="shared" ref="H664:H871" si="473">F664/10</f>
         <v>5.2200000000000006</v>
       </c>
       <c r="I664" s="3" t="s">
@@ -23032,7 +23041,7 @@
         <v>46.7</v>
       </c>
       <c r="G665" s="2">
-        <f t="shared" ref="G665:G747" si="474">E665/10</f>
+        <f t="shared" ref="G665:G871" si="474">E665/10</f>
         <v>4.3899999999999997</v>
       </c>
       <c r="H665" s="2">
@@ -25833,6 +25842,4286 @@
       <c r="J747" s="2">
         <v>136813</v>
       </c>
+    </row>
+    <row r="748" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A748" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B748" s="2">
+        <v>13</v>
+      </c>
+      <c r="C748" s="2">
+        <v>1</v>
+      </c>
+      <c r="D748" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="E748" s="2">
+        <v>48.7</v>
+      </c>
+      <c r="F748" s="2">
+        <v>57.9</v>
+      </c>
+      <c r="G748" s="2">
+        <f t="shared" si="474"/>
+        <v>4.87</v>
+      </c>
+      <c r="H748" s="2">
+        <f t="shared" si="473"/>
+        <v>5.79</v>
+      </c>
+      <c r="I748" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J748" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="749" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A749" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B749" s="2">
+        <v>13</v>
+      </c>
+      <c r="C749" s="2">
+        <v>2</v>
+      </c>
+      <c r="D749" s="2">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="E749" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="F749" s="2">
+        <v>55.9</v>
+      </c>
+      <c r="G749" s="2">
+        <f t="shared" si="474"/>
+        <v>4.75</v>
+      </c>
+      <c r="H749" s="2">
+        <f t="shared" si="473"/>
+        <v>5.59</v>
+      </c>
+      <c r="I749" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J749" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="750" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A750" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B750" s="2">
+        <v>13</v>
+      </c>
+      <c r="C750" s="2">
+        <v>3</v>
+      </c>
+      <c r="D750" s="2">
+        <v>0.754</v>
+      </c>
+      <c r="E750" s="2">
+        <v>39.6</v>
+      </c>
+      <c r="F750" s="2">
+        <v>46.1</v>
+      </c>
+      <c r="G750" s="2">
+        <f t="shared" si="474"/>
+        <v>3.96</v>
+      </c>
+      <c r="H750" s="2">
+        <f t="shared" si="473"/>
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="I750" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J750" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="751" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A751" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B751" s="2">
+        <v>13</v>
+      </c>
+      <c r="C751" s="2">
+        <v>4</v>
+      </c>
+      <c r="D751" s="2">
+        <v>1.738</v>
+      </c>
+      <c r="E751" s="2">
+        <v>50.2</v>
+      </c>
+      <c r="F751" s="2">
+        <v>59</v>
+      </c>
+      <c r="G751" s="2">
+        <f t="shared" si="474"/>
+        <v>5.0200000000000005</v>
+      </c>
+      <c r="H751" s="2">
+        <f t="shared" si="473"/>
+        <v>5.9</v>
+      </c>
+      <c r="I751" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J751" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="752" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A752" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B752" s="2">
+        <v>13</v>
+      </c>
+      <c r="C752" s="2">
+        <v>5</v>
+      </c>
+      <c r="D752" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="E752" s="2">
+        <v>39</v>
+      </c>
+      <c r="F752" s="2">
+        <v>46.7</v>
+      </c>
+      <c r="G752" s="2">
+        <f t="shared" si="474"/>
+        <v>3.9</v>
+      </c>
+      <c r="H752" s="2">
+        <f t="shared" si="473"/>
+        <v>4.67</v>
+      </c>
+      <c r="I752" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J752" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="753" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A753" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B753" s="2">
+        <v>13</v>
+      </c>
+      <c r="C753" s="2">
+        <v>6</v>
+      </c>
+      <c r="D753" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="E753" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="F753" s="2">
+        <v>49.1</v>
+      </c>
+      <c r="G753" s="2">
+        <f t="shared" si="474"/>
+        <v>4.17</v>
+      </c>
+      <c r="H753" s="2">
+        <f t="shared" si="473"/>
+        <v>4.91</v>
+      </c>
+      <c r="I753" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J753" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="754" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A754" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B754" s="2">
+        <v>13</v>
+      </c>
+      <c r="C754" s="2">
+        <v>7</v>
+      </c>
+      <c r="D754" s="2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E754" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="F754" s="2">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="G754" s="2">
+        <f t="shared" si="474"/>
+        <v>3.17</v>
+      </c>
+      <c r="H754" s="2">
+        <f t="shared" si="473"/>
+        <v>3.72</v>
+      </c>
+      <c r="I754" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J754" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="755" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A755" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B755" s="2">
+        <v>13</v>
+      </c>
+      <c r="C755" s="2">
+        <v>8</v>
+      </c>
+      <c r="D755" s="2">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="E755" s="2">
+        <v>47</v>
+      </c>
+      <c r="F755" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="G755" s="2">
+        <f t="shared" si="474"/>
+        <v>4.7</v>
+      </c>
+      <c r="H755" s="2">
+        <f t="shared" si="473"/>
+        <v>5.65</v>
+      </c>
+      <c r="I755" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J755" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="756" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A756" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B756" s="2">
+        <v>13</v>
+      </c>
+      <c r="C756" s="2">
+        <v>9</v>
+      </c>
+      <c r="D756" s="2">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="E756" s="2">
+        <v>45.4</v>
+      </c>
+      <c r="F756" s="2">
+        <v>53</v>
+      </c>
+      <c r="G756" s="2">
+        <f t="shared" si="474"/>
+        <v>4.54</v>
+      </c>
+      <c r="H756" s="2">
+        <f t="shared" si="473"/>
+        <v>5.3</v>
+      </c>
+      <c r="I756" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J756" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="757" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A757" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B757" s="2">
+        <v>13</v>
+      </c>
+      <c r="C757" s="2">
+        <v>10</v>
+      </c>
+      <c r="D757" s="2">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="E757" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="F757" s="2">
+        <v>50.1</v>
+      </c>
+      <c r="G757" s="2">
+        <f t="shared" si="474"/>
+        <v>4.17</v>
+      </c>
+      <c r="H757" s="2">
+        <f t="shared" si="473"/>
+        <v>5.01</v>
+      </c>
+      <c r="I757" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J757" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="758" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A758" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B758" s="2">
+        <v>13</v>
+      </c>
+      <c r="C758" s="2">
+        <v>11</v>
+      </c>
+      <c r="D758" s="2">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="E758" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="F758" s="2">
+        <v>46.6</v>
+      </c>
+      <c r="G758" s="2">
+        <f t="shared" si="474"/>
+        <v>3.95</v>
+      </c>
+      <c r="H758" s="2">
+        <f t="shared" si="473"/>
+        <v>4.66</v>
+      </c>
+      <c r="I758" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J758" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="759" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A759" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B759" s="2">
+        <v>13</v>
+      </c>
+      <c r="C759" s="2">
+        <v>12</v>
+      </c>
+      <c r="D759" s="2">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="E759" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="F759" s="2">
+        <v>49.9</v>
+      </c>
+      <c r="G759" s="2">
+        <f t="shared" si="474"/>
+        <v>4.17</v>
+      </c>
+      <c r="H759" s="2">
+        <f t="shared" si="473"/>
+        <v>4.99</v>
+      </c>
+      <c r="I759" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J759" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="760" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A760" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B760" s="2">
+        <v>13</v>
+      </c>
+      <c r="C760" s="2">
+        <v>13</v>
+      </c>
+      <c r="D760" s="2">
+        <v>1.1779999999999999</v>
+      </c>
+      <c r="E760" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="F760" s="2">
+        <v>53.9</v>
+      </c>
+      <c r="G760" s="2">
+        <f t="shared" si="474"/>
+        <v>4.55</v>
+      </c>
+      <c r="H760" s="2">
+        <f t="shared" si="473"/>
+        <v>5.39</v>
+      </c>
+      <c r="I760" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J760" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="761" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A761" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B761" s="2">
+        <v>13</v>
+      </c>
+      <c r="C761" s="2">
+        <v>14</v>
+      </c>
+      <c r="D761" s="2">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E761" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="F761" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="G761" s="2">
+        <f t="shared" si="474"/>
+        <v>4.05</v>
+      </c>
+      <c r="H761" s="2">
+        <f t="shared" si="473"/>
+        <v>4.7700000000000005</v>
+      </c>
+      <c r="I761" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J761" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="762" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A762" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B762" s="2">
+        <v>13</v>
+      </c>
+      <c r="C762" s="2">
+        <v>15</v>
+      </c>
+      <c r="D762" s="2">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E762" s="2">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="F762" s="2">
+        <v>38.1</v>
+      </c>
+      <c r="G762" s="2">
+        <f t="shared" si="474"/>
+        <v>3.3200000000000003</v>
+      </c>
+      <c r="H762" s="2">
+        <f t="shared" si="473"/>
+        <v>3.81</v>
+      </c>
+      <c r="I762" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J762" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="763" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A763" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B763" s="2">
+        <v>13</v>
+      </c>
+      <c r="C763" s="2">
+        <v>16</v>
+      </c>
+      <c r="D763" s="2">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="E763" s="2">
+        <v>42.6</v>
+      </c>
+      <c r="F763" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="G763" s="2">
+        <f t="shared" si="474"/>
+        <v>4.26</v>
+      </c>
+      <c r="H763" s="2">
+        <f t="shared" si="473"/>
+        <v>5.12</v>
+      </c>
+      <c r="I763" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J763" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="764" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A764" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B764" s="2">
+        <v>13</v>
+      </c>
+      <c r="C764" s="2">
+        <v>17</v>
+      </c>
+      <c r="D764" s="2">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E764" s="2">
+        <v>39</v>
+      </c>
+      <c r="F764" s="2">
+        <v>44.9</v>
+      </c>
+      <c r="G764" s="2">
+        <f t="shared" si="474"/>
+        <v>3.9</v>
+      </c>
+      <c r="H764" s="2">
+        <f t="shared" si="473"/>
+        <v>4.49</v>
+      </c>
+      <c r="I764" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J764" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="765" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A765" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B765" s="2">
+        <v>13</v>
+      </c>
+      <c r="C765" s="2">
+        <v>18</v>
+      </c>
+      <c r="D765" s="2">
+        <v>1.266</v>
+      </c>
+      <c r="E765" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="F765" s="2">
+        <v>53.5</v>
+      </c>
+      <c r="G765" s="2">
+        <f t="shared" si="474"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="H765" s="2">
+        <f t="shared" si="473"/>
+        <v>5.35</v>
+      </c>
+      <c r="I765" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J765" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="766" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A766" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B766" s="2">
+        <v>13</v>
+      </c>
+      <c r="C766" s="2">
+        <v>19</v>
+      </c>
+      <c r="D766" s="2">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="E766" s="2">
+        <v>42.4</v>
+      </c>
+      <c r="F766" s="2">
+        <v>49.9</v>
+      </c>
+      <c r="G766" s="2">
+        <f t="shared" si="474"/>
+        <v>4.24</v>
+      </c>
+      <c r="H766" s="2">
+        <f t="shared" si="473"/>
+        <v>4.99</v>
+      </c>
+      <c r="I766" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J766" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="767" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A767" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B767" s="2">
+        <v>13</v>
+      </c>
+      <c r="C767" s="2">
+        <v>20</v>
+      </c>
+      <c r="D767" s="2">
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="E767" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="F767" s="2">
+        <v>53.9</v>
+      </c>
+      <c r="G767" s="2">
+        <f t="shared" si="474"/>
+        <v>4.55</v>
+      </c>
+      <c r="H767" s="2">
+        <f t="shared" si="473"/>
+        <v>5.39</v>
+      </c>
+      <c r="I767" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J767" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="768" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A768" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B768" s="2">
+        <v>13</v>
+      </c>
+      <c r="C768" s="2">
+        <v>21</v>
+      </c>
+      <c r="D768" s="2">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="E768" s="2">
+        <v>42.7</v>
+      </c>
+      <c r="F768" s="2">
+        <v>49.9</v>
+      </c>
+      <c r="G768" s="2">
+        <f t="shared" si="474"/>
+        <v>4.2700000000000005</v>
+      </c>
+      <c r="H768" s="2">
+        <f t="shared" si="473"/>
+        <v>4.99</v>
+      </c>
+      <c r="I768" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J768" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="769" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A769" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B769" s="2">
+        <v>13</v>
+      </c>
+      <c r="C769" s="2">
+        <v>22</v>
+      </c>
+      <c r="D769" s="2">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="E769" s="2">
+        <v>44.3</v>
+      </c>
+      <c r="F769" s="2">
+        <v>52.8</v>
+      </c>
+      <c r="G769" s="2">
+        <f t="shared" si="474"/>
+        <v>4.43</v>
+      </c>
+      <c r="H769" s="2">
+        <f t="shared" si="473"/>
+        <v>5.2799999999999994</v>
+      </c>
+      <c r="I769" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J769" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="770" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A770" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B770" s="2">
+        <v>13</v>
+      </c>
+      <c r="C770" s="2">
+        <v>23</v>
+      </c>
+      <c r="D770" s="2">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="E770" s="2">
+        <v>42</v>
+      </c>
+      <c r="F770" s="2">
+        <v>49.1</v>
+      </c>
+      <c r="G770" s="2">
+        <f t="shared" si="474"/>
+        <v>4.2</v>
+      </c>
+      <c r="H770" s="2">
+        <f t="shared" si="473"/>
+        <v>4.91</v>
+      </c>
+      <c r="I770" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J770" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="771" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A771" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B771" s="2">
+        <v>13</v>
+      </c>
+      <c r="C771" s="2">
+        <v>24</v>
+      </c>
+      <c r="D771" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="E771" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="F771" s="2">
+        <v>47.9</v>
+      </c>
+      <c r="G771" s="2">
+        <f t="shared" si="474"/>
+        <v>4.2299999999999995</v>
+      </c>
+      <c r="H771" s="2">
+        <f t="shared" si="473"/>
+        <v>4.79</v>
+      </c>
+      <c r="I771" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J771" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="772" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A772" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B772" s="2">
+        <v>13</v>
+      </c>
+      <c r="C772" s="2">
+        <v>25</v>
+      </c>
+      <c r="D772" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="E772" s="2">
+        <v>37.4</v>
+      </c>
+      <c r="F772" s="2">
+        <v>44.7</v>
+      </c>
+      <c r="G772" s="2">
+        <f t="shared" si="474"/>
+        <v>3.7399999999999998</v>
+      </c>
+      <c r="H772" s="2">
+        <f t="shared" si="473"/>
+        <v>4.4700000000000006</v>
+      </c>
+      <c r="I772" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J772" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="773" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A773" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B773" s="2">
+        <v>13</v>
+      </c>
+      <c r="C773" s="2">
+        <v>26</v>
+      </c>
+      <c r="D773" s="2">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="E773" s="2">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F773" s="2">
+        <v>44.5</v>
+      </c>
+      <c r="G773" s="2">
+        <f t="shared" si="474"/>
+        <v>3.88</v>
+      </c>
+      <c r="H773" s="2">
+        <f t="shared" si="473"/>
+        <v>4.45</v>
+      </c>
+      <c r="I773" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J773" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="774" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A774" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B774" s="2">
+        <v>13</v>
+      </c>
+      <c r="C774" s="2">
+        <v>27</v>
+      </c>
+      <c r="D774" s="2">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E774" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="F774" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="G774" s="2">
+        <f t="shared" si="474"/>
+        <v>4.07</v>
+      </c>
+      <c r="H774" s="2">
+        <f t="shared" si="473"/>
+        <v>4.75</v>
+      </c>
+      <c r="I774" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J774" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="775" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A775" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B775" s="2">
+        <v>13</v>
+      </c>
+      <c r="C775" s="2">
+        <v>28</v>
+      </c>
+      <c r="D775" s="2">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="E775" s="2">
+        <v>37.4</v>
+      </c>
+      <c r="F775" s="2">
+        <v>44.6</v>
+      </c>
+      <c r="G775" s="2">
+        <f t="shared" si="474"/>
+        <v>3.7399999999999998</v>
+      </c>
+      <c r="H775" s="2">
+        <f t="shared" si="473"/>
+        <v>4.46</v>
+      </c>
+      <c r="I775" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J775" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="776" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A776" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B776" s="2">
+        <v>13</v>
+      </c>
+      <c r="C776" s="2">
+        <v>29</v>
+      </c>
+      <c r="D776" s="2">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="E776" s="2">
+        <v>31.4</v>
+      </c>
+      <c r="F776" s="2">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G776" s="2">
+        <f t="shared" si="474"/>
+        <v>3.1399999999999997</v>
+      </c>
+      <c r="H776" s="2">
+        <f t="shared" si="473"/>
+        <v>3.5200000000000005</v>
+      </c>
+      <c r="I776" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J776" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="777" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A777" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B777" s="2">
+        <v>13</v>
+      </c>
+      <c r="C777" s="2">
+        <v>30</v>
+      </c>
+      <c r="D777" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="E777" s="2">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F777" s="2">
+        <v>46.3</v>
+      </c>
+      <c r="G777" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0299999999999994</v>
+      </c>
+      <c r="H777" s="2">
+        <f t="shared" si="473"/>
+        <v>4.63</v>
+      </c>
+      <c r="I777" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J777" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="778" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A778" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B778" s="2">
+        <v>13</v>
+      </c>
+      <c r="C778" s="2">
+        <v>31</v>
+      </c>
+      <c r="D778" s="2">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="E778" s="2">
+        <v>45</v>
+      </c>
+      <c r="F778" s="2">
+        <v>52.4</v>
+      </c>
+      <c r="G778" s="2">
+        <f t="shared" si="474"/>
+        <v>4.5</v>
+      </c>
+      <c r="H778" s="2">
+        <f t="shared" si="473"/>
+        <v>5.24</v>
+      </c>
+      <c r="I778" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J778" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="779" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A779" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B779" s="2">
+        <v>13</v>
+      </c>
+      <c r="C779" s="2">
+        <v>32</v>
+      </c>
+      <c r="D779" s="2">
+        <v>1.054</v>
+      </c>
+      <c r="E779" s="2">
+        <v>42.5</v>
+      </c>
+      <c r="F779" s="2">
+        <v>50.7</v>
+      </c>
+      <c r="G779" s="2">
+        <f t="shared" si="474"/>
+        <v>4.25</v>
+      </c>
+      <c r="H779" s="2">
+        <f t="shared" si="473"/>
+        <v>5.07</v>
+      </c>
+      <c r="I779" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J779" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="780" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A780" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B780" s="2">
+        <v>13</v>
+      </c>
+      <c r="C780" s="2">
+        <v>33</v>
+      </c>
+      <c r="D780" s="2">
+        <v>1.216</v>
+      </c>
+      <c r="E780" s="2">
+        <v>45.8</v>
+      </c>
+      <c r="F780" s="2">
+        <v>53.9</v>
+      </c>
+      <c r="G780" s="2">
+        <f t="shared" si="474"/>
+        <v>4.58</v>
+      </c>
+      <c r="H780" s="2">
+        <f t="shared" si="473"/>
+        <v>5.39</v>
+      </c>
+      <c r="I780" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J780" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="781" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A781" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B781" s="2">
+        <v>13</v>
+      </c>
+      <c r="C781" s="2">
+        <v>34</v>
+      </c>
+      <c r="D781" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="E781" s="2">
+        <v>42.9</v>
+      </c>
+      <c r="F781" s="2">
+        <v>50.1</v>
+      </c>
+      <c r="G781" s="2">
+        <f t="shared" si="474"/>
+        <v>4.29</v>
+      </c>
+      <c r="H781" s="2">
+        <f t="shared" si="473"/>
+        <v>5.01</v>
+      </c>
+      <c r="I781" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J781" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="782" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A782" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B782" s="2">
+        <v>13</v>
+      </c>
+      <c r="C782" s="2">
+        <v>35</v>
+      </c>
+      <c r="D782" s="2">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="E782" s="2">
+        <v>41</v>
+      </c>
+      <c r="F782" s="2">
+        <v>50.1</v>
+      </c>
+      <c r="G782" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H782" s="2">
+        <f t="shared" si="473"/>
+        <v>5.01</v>
+      </c>
+      <c r="I782" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J782" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="783" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A783" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B783" s="2">
+        <v>13</v>
+      </c>
+      <c r="C783" s="2">
+        <v>36</v>
+      </c>
+      <c r="D783" s="2">
+        <v>1.181</v>
+      </c>
+      <c r="E783" s="2">
+        <v>44.9</v>
+      </c>
+      <c r="F783" s="2">
+        <v>52.8</v>
+      </c>
+      <c r="G783" s="2">
+        <f t="shared" si="474"/>
+        <v>4.49</v>
+      </c>
+      <c r="H783" s="2">
+        <f t="shared" si="473"/>
+        <v>5.2799999999999994</v>
+      </c>
+      <c r="I783" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J783" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="784" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A784" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B784" s="2">
+        <v>13</v>
+      </c>
+      <c r="C784" s="2">
+        <v>37</v>
+      </c>
+      <c r="D784" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E784" s="2">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F784" s="2">
+        <v>45.9</v>
+      </c>
+      <c r="G784" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0299999999999994</v>
+      </c>
+      <c r="H784" s="2">
+        <f t="shared" si="473"/>
+        <v>4.59</v>
+      </c>
+      <c r="I784" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J784" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="785" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A785" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B785" s="2">
+        <v>13</v>
+      </c>
+      <c r="C785" s="2">
+        <v>38</v>
+      </c>
+      <c r="D785" s="2">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="E785" s="2">
+        <v>40.9</v>
+      </c>
+      <c r="F785" s="2">
+        <v>48.1</v>
+      </c>
+      <c r="G785" s="2">
+        <f t="shared" si="474"/>
+        <v>4.09</v>
+      </c>
+      <c r="H785" s="2">
+        <f t="shared" si="473"/>
+        <v>4.8100000000000005</v>
+      </c>
+      <c r="I785" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J785" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="786" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A786" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B786" s="2">
+        <v>13</v>
+      </c>
+      <c r="C786" s="2">
+        <v>39</v>
+      </c>
+      <c r="D786" s="2">
+        <v>1.3080000000000001</v>
+      </c>
+      <c r="E786" s="2">
+        <v>46.3</v>
+      </c>
+      <c r="F786" s="2">
+        <v>54.7</v>
+      </c>
+      <c r="G786" s="2">
+        <f t="shared" si="474"/>
+        <v>4.63</v>
+      </c>
+      <c r="H786" s="2">
+        <f t="shared" si="473"/>
+        <v>5.4700000000000006</v>
+      </c>
+      <c r="I786" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J786" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="787" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A787" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B787" s="2">
+        <v>13</v>
+      </c>
+      <c r="C787" s="2">
+        <v>40</v>
+      </c>
+      <c r="D787" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E787" s="2">
+        <v>41.3</v>
+      </c>
+      <c r="F787" s="2">
+        <v>48.4</v>
+      </c>
+      <c r="G787" s="2">
+        <f t="shared" si="474"/>
+        <v>4.13</v>
+      </c>
+      <c r="H787" s="2">
+        <f t="shared" si="473"/>
+        <v>4.84</v>
+      </c>
+      <c r="I787" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J787" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="788" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A788" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B788" s="2">
+        <v>13</v>
+      </c>
+      <c r="C788" s="2">
+        <v>41</v>
+      </c>
+      <c r="D788" s="2">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="E788" s="2">
+        <v>39.6</v>
+      </c>
+      <c r="F788" s="2">
+        <v>46</v>
+      </c>
+      <c r="G788" s="2">
+        <f t="shared" si="474"/>
+        <v>3.96</v>
+      </c>
+      <c r="H788" s="2">
+        <f t="shared" si="473"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I788" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J788" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="789" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A789" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B789" s="2">
+        <v>13</v>
+      </c>
+      <c r="C789" s="2">
+        <v>42</v>
+      </c>
+      <c r="D789" s="2">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="E789" s="2">
+        <v>41</v>
+      </c>
+      <c r="F789" s="2">
+        <v>47.4</v>
+      </c>
+      <c r="G789" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H789" s="2">
+        <f t="shared" si="473"/>
+        <v>4.74</v>
+      </c>
+      <c r="I789" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J789" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="790" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A790" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B790" s="2">
+        <v>13</v>
+      </c>
+      <c r="C790" s="2">
+        <v>43</v>
+      </c>
+      <c r="D790" s="2">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="E790" s="2">
+        <v>36.5</v>
+      </c>
+      <c r="F790" s="2">
+        <v>43</v>
+      </c>
+      <c r="G790" s="2">
+        <f t="shared" si="474"/>
+        <v>3.65</v>
+      </c>
+      <c r="H790" s="2">
+        <f t="shared" si="473"/>
+        <v>4.3</v>
+      </c>
+      <c r="I790" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J790" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="791" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A791" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B791" s="2">
+        <v>13</v>
+      </c>
+      <c r="C791" s="2">
+        <v>44</v>
+      </c>
+      <c r="D791" s="2">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="E791" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="F791" s="2">
+        <v>38.4</v>
+      </c>
+      <c r="G791" s="2">
+        <f t="shared" si="474"/>
+        <v>3.08</v>
+      </c>
+      <c r="H791" s="2">
+        <f t="shared" si="473"/>
+        <v>3.84</v>
+      </c>
+      <c r="I791" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J791" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="792" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A792" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B792" s="2">
+        <v>13</v>
+      </c>
+      <c r="C792" s="2">
+        <v>45</v>
+      </c>
+      <c r="D792" s="2">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="E792" s="2">
+        <v>41</v>
+      </c>
+      <c r="F792" s="2">
+        <v>52.4</v>
+      </c>
+      <c r="G792" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H792" s="2">
+        <f t="shared" si="473"/>
+        <v>5.24</v>
+      </c>
+      <c r="I792" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J792" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="793" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A793" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B793" s="2">
+        <v>13</v>
+      </c>
+      <c r="C793" s="2">
+        <v>46</v>
+      </c>
+      <c r="D793" s="2">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="E793" s="2">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="F793" s="2">
+        <v>46.4</v>
+      </c>
+      <c r="G793" s="2">
+        <f t="shared" si="474"/>
+        <v>3.9299999999999997</v>
+      </c>
+      <c r="H793" s="2">
+        <f t="shared" si="473"/>
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I793" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J793" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="794" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A794" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B794" s="2">
+        <v>13</v>
+      </c>
+      <c r="C794" s="2">
+        <v>47</v>
+      </c>
+      <c r="D794" s="2">
+        <v>1.1830000000000001</v>
+      </c>
+      <c r="E794" s="2">
+        <v>43.2</v>
+      </c>
+      <c r="F794" s="2">
+        <v>51.1</v>
+      </c>
+      <c r="G794" s="2">
+        <f t="shared" si="474"/>
+        <v>4.32</v>
+      </c>
+      <c r="H794" s="2">
+        <f t="shared" si="473"/>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="I794" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J794" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="795" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A795" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B795" s="2">
+        <v>13</v>
+      </c>
+      <c r="C795" s="2">
+        <v>48</v>
+      </c>
+      <c r="D795" s="2">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="E795" s="2">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F795" s="2">
+        <v>42.9</v>
+      </c>
+      <c r="G795" s="2">
+        <f t="shared" si="474"/>
+        <v>3.53</v>
+      </c>
+      <c r="H795" s="2">
+        <f t="shared" si="473"/>
+        <v>4.29</v>
+      </c>
+      <c r="I795" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J795" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="796" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A796" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B796" s="2">
+        <v>13</v>
+      </c>
+      <c r="C796" s="2">
+        <v>49</v>
+      </c>
+      <c r="D796" s="2">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E796" s="2">
+        <v>31.3</v>
+      </c>
+      <c r="F796" s="2">
+        <v>36.9</v>
+      </c>
+      <c r="G796" s="2">
+        <f t="shared" si="474"/>
+        <v>3.13</v>
+      </c>
+      <c r="H796" s="2">
+        <f t="shared" si="473"/>
+        <v>3.69</v>
+      </c>
+      <c r="I796" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J796" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="797" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A797" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B797" s="2">
+        <v>13</v>
+      </c>
+      <c r="C797" s="2">
+        <v>50</v>
+      </c>
+      <c r="D797" s="2">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="E797" s="2">
+        <v>43.9</v>
+      </c>
+      <c r="F797" s="2">
+        <v>51.9</v>
+      </c>
+      <c r="G797" s="2">
+        <f t="shared" si="474"/>
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="H797" s="2">
+        <f t="shared" si="473"/>
+        <v>5.1899999999999995</v>
+      </c>
+      <c r="I797" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J797" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="798" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A798" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B798" s="2">
+        <v>13</v>
+      </c>
+      <c r="C798" s="2">
+        <v>51</v>
+      </c>
+      <c r="D798" s="2">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E798" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="F798" s="2">
+        <v>39.1</v>
+      </c>
+      <c r="G798" s="2">
+        <f t="shared" si="474"/>
+        <v>3.35</v>
+      </c>
+      <c r="H798" s="2">
+        <f t="shared" si="473"/>
+        <v>3.91</v>
+      </c>
+      <c r="I798" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J798" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="799" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A799" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B799" s="2">
+        <v>13</v>
+      </c>
+      <c r="C799" s="2">
+        <v>52</v>
+      </c>
+      <c r="D799" s="2">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="E799" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="F799" s="2">
+        <v>44.6</v>
+      </c>
+      <c r="G799" s="2">
+        <f t="shared" si="474"/>
+        <v>4.05</v>
+      </c>
+      <c r="H799" s="2">
+        <f t="shared" si="473"/>
+        <v>4.46</v>
+      </c>
+      <c r="I799" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J799" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="800" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A800" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B800" s="2">
+        <v>13</v>
+      </c>
+      <c r="C800" s="2">
+        <v>53</v>
+      </c>
+      <c r="D800" s="2">
+        <v>1.1870000000000001</v>
+      </c>
+      <c r="E800" s="2">
+        <v>44.8</v>
+      </c>
+      <c r="F800" s="2">
+        <v>53.6</v>
+      </c>
+      <c r="G800" s="2">
+        <f t="shared" si="474"/>
+        <v>4.4799999999999995</v>
+      </c>
+      <c r="H800" s="2">
+        <f t="shared" si="473"/>
+        <v>5.36</v>
+      </c>
+      <c r="I800" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J800" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="801" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A801" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B801" s="2">
+        <v>13</v>
+      </c>
+      <c r="C801" s="2">
+        <v>54</v>
+      </c>
+      <c r="D801" s="2">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="E801" s="2">
+        <v>38</v>
+      </c>
+      <c r="F801" s="2">
+        <v>43.8</v>
+      </c>
+      <c r="G801" s="2">
+        <f t="shared" si="474"/>
+        <v>3.8</v>
+      </c>
+      <c r="H801" s="2">
+        <f t="shared" si="473"/>
+        <v>4.38</v>
+      </c>
+      <c r="I801" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J801" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="802" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A802" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B802" s="2">
+        <v>13</v>
+      </c>
+      <c r="C802" s="2">
+        <v>55</v>
+      </c>
+      <c r="D802" s="2">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E802" s="2">
+        <v>43.7</v>
+      </c>
+      <c r="F802" s="2">
+        <v>51.1</v>
+      </c>
+      <c r="G802" s="2">
+        <f t="shared" si="474"/>
+        <v>4.37</v>
+      </c>
+      <c r="H802" s="2">
+        <f t="shared" si="473"/>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="I802" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J802" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="803" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A803" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B803" s="2">
+        <v>13</v>
+      </c>
+      <c r="C803" s="2">
+        <v>56</v>
+      </c>
+      <c r="D803" s="2">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="E803" s="2">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="F803" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="G803" s="2">
+        <f t="shared" si="474"/>
+        <v>3.5700000000000003</v>
+      </c>
+      <c r="H803" s="2">
+        <f t="shared" si="473"/>
+        <v>4.2299999999999995</v>
+      </c>
+      <c r="I803" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J803" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="804" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A804" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B804" s="2">
+        <v>13</v>
+      </c>
+      <c r="C804" s="2">
+        <v>57</v>
+      </c>
+      <c r="D804" s="2">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="E804" s="2">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="F804" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="G804" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0200000000000005</v>
+      </c>
+      <c r="H804" s="2">
+        <f t="shared" si="473"/>
+        <v>4.7700000000000005</v>
+      </c>
+      <c r="I804" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J804" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="805" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A805" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B805" s="2">
+        <v>13</v>
+      </c>
+      <c r="C805" s="2">
+        <v>58</v>
+      </c>
+      <c r="D805" s="2">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="E805" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="F805" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="G805" s="2">
+        <f t="shared" si="474"/>
+        <v>4.07</v>
+      </c>
+      <c r="H805" s="2">
+        <f t="shared" si="473"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="I805" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J805" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="806" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A806" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B806" s="2">
+        <v>13</v>
+      </c>
+      <c r="C806" s="2">
+        <v>59</v>
+      </c>
+      <c r="D806" s="2">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="E806" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="F806" s="2">
+        <v>46.6</v>
+      </c>
+      <c r="G806" s="2">
+        <f t="shared" si="474"/>
+        <v>4.05</v>
+      </c>
+      <c r="H806" s="2">
+        <f t="shared" si="473"/>
+        <v>4.66</v>
+      </c>
+      <c r="I806" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J806" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="807" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A807" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B807" s="2">
+        <v>13</v>
+      </c>
+      <c r="C807" s="2">
+        <v>60</v>
+      </c>
+      <c r="D807" s="2">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="E807" s="2">
+        <v>42.6</v>
+      </c>
+      <c r="F807" s="2">
+        <v>50.2</v>
+      </c>
+      <c r="G807" s="2">
+        <f t="shared" si="474"/>
+        <v>4.26</v>
+      </c>
+      <c r="H807" s="2">
+        <f t="shared" si="473"/>
+        <v>5.0200000000000005</v>
+      </c>
+      <c r="I807" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J807" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="808" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A808" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B808" s="2">
+        <v>13</v>
+      </c>
+      <c r="C808" s="2">
+        <v>61</v>
+      </c>
+      <c r="D808" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="E808" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="F808" s="2">
+        <v>48.8</v>
+      </c>
+      <c r="G808" s="2">
+        <f t="shared" si="474"/>
+        <v>4.07</v>
+      </c>
+      <c r="H808" s="2">
+        <f t="shared" si="473"/>
+        <v>4.88</v>
+      </c>
+      <c r="I808" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J808" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="809" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A809" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B809" s="2">
+        <v>13</v>
+      </c>
+      <c r="C809" s="2">
+        <v>62</v>
+      </c>
+      <c r="D809" s="2">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E809" s="2">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F809" s="2">
+        <v>45.6</v>
+      </c>
+      <c r="G809" s="2">
+        <f t="shared" si="474"/>
+        <v>4.0299999999999994</v>
+      </c>
+      <c r="H809" s="2">
+        <f t="shared" si="473"/>
+        <v>4.5600000000000005</v>
+      </c>
+      <c r="I809" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J809" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="810" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A810" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B810" s="2">
+        <v>13</v>
+      </c>
+      <c r="C810" s="2">
+        <v>63</v>
+      </c>
+      <c r="D810" s="2">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E810" s="2">
+        <v>41.5</v>
+      </c>
+      <c r="F810" s="2">
+        <v>49.2</v>
+      </c>
+      <c r="G810" s="2">
+        <f t="shared" si="474"/>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="H810" s="2">
+        <f t="shared" si="473"/>
+        <v>4.92</v>
+      </c>
+      <c r="I810" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J810" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="811" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A811" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B811" s="2">
+        <v>13</v>
+      </c>
+      <c r="C811" s="2">
+        <v>64</v>
+      </c>
+      <c r="D811" s="2">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="E811" s="2">
+        <v>42.9</v>
+      </c>
+      <c r="F811" s="2">
+        <v>50.9</v>
+      </c>
+      <c r="G811" s="2">
+        <f t="shared" si="474"/>
+        <v>4.29</v>
+      </c>
+      <c r="H811" s="2">
+        <f t="shared" si="473"/>
+        <v>5.09</v>
+      </c>
+      <c r="I811" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J811" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="812" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A812" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B812" s="2">
+        <v>13</v>
+      </c>
+      <c r="C812" s="2">
+        <v>65</v>
+      </c>
+      <c r="D812" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="E812" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F812" s="2">
+        <v>43.6</v>
+      </c>
+      <c r="G812" s="2">
+        <f t="shared" si="474"/>
+        <v>3.6799999999999997</v>
+      </c>
+      <c r="H812" s="2">
+        <f t="shared" si="473"/>
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="I812" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J812" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="813" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A813" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B813" s="2">
+        <v>13</v>
+      </c>
+      <c r="C813" s="2">
+        <v>66</v>
+      </c>
+      <c r="D813" s="2">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="E813" s="2">
+        <v>44.3</v>
+      </c>
+      <c r="F813" s="2">
+        <v>53</v>
+      </c>
+      <c r="G813" s="2">
+        <f t="shared" si="474"/>
+        <v>4.43</v>
+      </c>
+      <c r="H813" s="2">
+        <f t="shared" si="473"/>
+        <v>5.3</v>
+      </c>
+      <c r="I813" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J813" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="814" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A814" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B814" s="2">
+        <v>13</v>
+      </c>
+      <c r="C814" s="2">
+        <v>67</v>
+      </c>
+      <c r="D814" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="E814" s="2">
+        <v>36.4</v>
+      </c>
+      <c r="F814" s="2">
+        <v>42.4</v>
+      </c>
+      <c r="G814" s="2">
+        <f t="shared" si="474"/>
+        <v>3.6399999999999997</v>
+      </c>
+      <c r="H814" s="2">
+        <f t="shared" si="473"/>
+        <v>4.24</v>
+      </c>
+      <c r="I814" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J814" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="815" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A815" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B815" s="2">
+        <v>13</v>
+      </c>
+      <c r="C815" s="2">
+        <v>68</v>
+      </c>
+      <c r="D815" s="2">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E815" s="2">
+        <v>29</v>
+      </c>
+      <c r="F815" s="2">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="G815" s="2">
+        <f t="shared" si="474"/>
+        <v>2.9</v>
+      </c>
+      <c r="H815" s="2">
+        <f t="shared" si="473"/>
+        <v>3.3200000000000003</v>
+      </c>
+      <c r="I815" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J815" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="816" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A816" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B816" s="2">
+        <v>13</v>
+      </c>
+      <c r="C816" s="2">
+        <v>69</v>
+      </c>
+      <c r="D816" s="2">
+        <v>0.311</v>
+      </c>
+      <c r="E816" s="2">
+        <v>31</v>
+      </c>
+      <c r="F816" s="2">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G816" s="2">
+        <f t="shared" si="474"/>
+        <v>3.1</v>
+      </c>
+      <c r="H816" s="2">
+        <f t="shared" si="473"/>
+        <v>3.5799999999999996</v>
+      </c>
+      <c r="I816" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J816" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="817" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A817" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B817" s="2">
+        <v>13</v>
+      </c>
+      <c r="C817" s="2">
+        <v>70</v>
+      </c>
+      <c r="D817" s="2">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="E817" s="2">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F817" s="2">
+        <v>43</v>
+      </c>
+      <c r="G817" s="2">
+        <f t="shared" si="474"/>
+        <v>3.72</v>
+      </c>
+      <c r="H817" s="2">
+        <f t="shared" si="473"/>
+        <v>4.3</v>
+      </c>
+      <c r="I817" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J817" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="818" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A818" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B818" s="2">
+        <v>13</v>
+      </c>
+      <c r="C818" s="2">
+        <v>71</v>
+      </c>
+      <c r="D818" s="2">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="E818" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="F818" s="2">
+        <v>46</v>
+      </c>
+      <c r="G818" s="2">
+        <f t="shared" si="474"/>
+        <v>4.05</v>
+      </c>
+      <c r="H818" s="2">
+        <f t="shared" si="473"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I818" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J818" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="819" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A819" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B819" s="2">
+        <v>13</v>
+      </c>
+      <c r="C819" s="2">
+        <v>72</v>
+      </c>
+      <c r="D819" s="2">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E819" s="2">
+        <v>39</v>
+      </c>
+      <c r="F819" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="G819" s="2">
+        <f t="shared" si="474"/>
+        <v>3.9</v>
+      </c>
+      <c r="H819" s="2">
+        <f t="shared" si="473"/>
+        <v>4.75</v>
+      </c>
+      <c r="I819" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J819" s="2">
+        <v>136807</v>
+      </c>
+    </row>
+    <row r="820" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A820" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B820" s="2">
+        <v>13</v>
+      </c>
+      <c r="C820" s="2">
+        <v>73</v>
+      </c>
+      <c r="D820" s="2">
+        <v>5.5389999999999997</v>
+      </c>
+      <c r="E820" s="2">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="F820" s="2">
+        <v>80.2</v>
+      </c>
+      <c r="G820" s="2">
+        <f t="shared" si="474"/>
+        <v>6.7900000000000009</v>
+      </c>
+      <c r="H820" s="2">
+        <f t="shared" si="473"/>
+        <v>8.02</v>
+      </c>
+      <c r="I820" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J820" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="821" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A821" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B821" s="2">
+        <v>13</v>
+      </c>
+      <c r="C821" s="2">
+        <v>74</v>
+      </c>
+      <c r="D821" s="2">
+        <v>5.73</v>
+      </c>
+      <c r="E821" s="2">
+        <v>65.7</v>
+      </c>
+      <c r="F821" s="2">
+        <v>82.4</v>
+      </c>
+      <c r="G821" s="2">
+        <f t="shared" si="474"/>
+        <v>6.57</v>
+      </c>
+      <c r="H821" s="2">
+        <f t="shared" si="473"/>
+        <v>8.24</v>
+      </c>
+      <c r="I821" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J821" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="822" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A822" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B822" s="2">
+        <v>13</v>
+      </c>
+      <c r="C822" s="2">
+        <v>75</v>
+      </c>
+      <c r="D822" s="2">
+        <v>9.2780000000000005</v>
+      </c>
+      <c r="E822" s="2">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="F822" s="2">
+        <v>96.1</v>
+      </c>
+      <c r="G822" s="2">
+        <f t="shared" si="474"/>
+        <v>7.69</v>
+      </c>
+      <c r="H822" s="2">
+        <f t="shared" si="473"/>
+        <v>9.61</v>
+      </c>
+      <c r="I822" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J822" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="823" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A823" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B823" s="2">
+        <v>13</v>
+      </c>
+      <c r="C823" s="2">
+        <v>76</v>
+      </c>
+      <c r="D823" s="2">
+        <v>5.08</v>
+      </c>
+      <c r="E823" s="2">
+        <v>64.8</v>
+      </c>
+      <c r="F823" s="2">
+        <v>79.8</v>
+      </c>
+      <c r="G823" s="2">
+        <f t="shared" si="474"/>
+        <v>6.4799999999999995</v>
+      </c>
+      <c r="H823" s="2">
+        <f t="shared" si="473"/>
+        <v>7.9799999999999995</v>
+      </c>
+      <c r="I823" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J823" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="824" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A824" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B824" s="2">
+        <v>13</v>
+      </c>
+      <c r="C824" s="2">
+        <v>77</v>
+      </c>
+      <c r="D824" s="2">
+        <v>7.5069999999999997</v>
+      </c>
+      <c r="E824" s="2">
+        <v>71.2</v>
+      </c>
+      <c r="F824" s="2">
+        <v>85.9</v>
+      </c>
+      <c r="G824" s="2">
+        <f t="shared" si="474"/>
+        <v>7.12</v>
+      </c>
+      <c r="H824" s="2">
+        <f t="shared" si="473"/>
+        <v>8.59</v>
+      </c>
+      <c r="I824" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J824" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="825" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A825" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B825" s="2">
+        <v>13</v>
+      </c>
+      <c r="C825" s="2">
+        <v>78</v>
+      </c>
+      <c r="D825" s="2">
+        <v>6.8940000000000001</v>
+      </c>
+      <c r="E825" s="2">
+        <v>74.2</v>
+      </c>
+      <c r="F825" s="2">
+        <v>89.6</v>
+      </c>
+      <c r="G825" s="2">
+        <f t="shared" si="474"/>
+        <v>7.42</v>
+      </c>
+      <c r="H825" s="2">
+        <f t="shared" si="473"/>
+        <v>8.9599999999999991</v>
+      </c>
+      <c r="I825" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J825" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="826" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A826" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B826" s="2">
+        <v>13</v>
+      </c>
+      <c r="C826" s="2">
+        <v>79</v>
+      </c>
+      <c r="D826" s="2">
+        <v>6.0620000000000003</v>
+      </c>
+      <c r="E826" s="2">
+        <v>68.5</v>
+      </c>
+      <c r="F826" s="2">
+        <v>84.7</v>
+      </c>
+      <c r="G826" s="2">
+        <f t="shared" si="474"/>
+        <v>6.85</v>
+      </c>
+      <c r="H826" s="2">
+        <f t="shared" si="473"/>
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="I826" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J826" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="827" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A827" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B827" s="2">
+        <v>13</v>
+      </c>
+      <c r="C827" s="2">
+        <v>80</v>
+      </c>
+      <c r="D827" s="2">
+        <v>0.496</v>
+      </c>
+      <c r="E827" s="2">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F827" s="2">
+        <v>39.9</v>
+      </c>
+      <c r="G827" s="2">
+        <f t="shared" si="474"/>
+        <v>3.4799999999999995</v>
+      </c>
+      <c r="H827" s="2">
+        <f t="shared" si="473"/>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="I827" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J827" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="828" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A828" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B828" s="2">
+        <v>13</v>
+      </c>
+      <c r="C828" s="2">
+        <v>81</v>
+      </c>
+      <c r="D828" s="2">
+        <v>8.1690000000000005</v>
+      </c>
+      <c r="E828" s="2">
+        <v>74.5</v>
+      </c>
+      <c r="F828" s="2">
+        <v>91.6</v>
+      </c>
+      <c r="G828" s="2">
+        <f t="shared" si="474"/>
+        <v>7.45</v>
+      </c>
+      <c r="H828" s="2">
+        <f t="shared" si="473"/>
+        <v>9.16</v>
+      </c>
+      <c r="I828" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J828" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="829" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A829" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B829" s="2">
+        <v>13</v>
+      </c>
+      <c r="C829" s="2">
+        <v>82</v>
+      </c>
+      <c r="D829" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="E829" s="2">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="F829" s="2">
+        <v>79.5</v>
+      </c>
+      <c r="G829" s="2">
+        <f t="shared" si="474"/>
+        <v>6.7900000000000009</v>
+      </c>
+      <c r="H829" s="2">
+        <f t="shared" si="473"/>
+        <v>7.95</v>
+      </c>
+      <c r="I829" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J829" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="830" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A830" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B830" s="2">
+        <v>13</v>
+      </c>
+      <c r="C830" s="2">
+        <v>83</v>
+      </c>
+      <c r="D830" s="2">
+        <v>3.56</v>
+      </c>
+      <c r="E830" s="2">
+        <v>58.8</v>
+      </c>
+      <c r="F830" s="2">
+        <v>71.3</v>
+      </c>
+      <c r="G830" s="2">
+        <f t="shared" si="474"/>
+        <v>5.88</v>
+      </c>
+      <c r="H830" s="2">
+        <f t="shared" si="473"/>
+        <v>7.13</v>
+      </c>
+      <c r="I830" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J830" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="831" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A831" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B831" s="2">
+        <v>13</v>
+      </c>
+      <c r="C831" s="2">
+        <v>84</v>
+      </c>
+      <c r="D831" s="2">
+        <v>3.0579999999999998</v>
+      </c>
+      <c r="E831" s="2">
+        <v>56.3</v>
+      </c>
+      <c r="F831" s="2">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="G831" s="2">
+        <f t="shared" si="474"/>
+        <v>5.63</v>
+      </c>
+      <c r="H831" s="2">
+        <f t="shared" si="473"/>
+        <v>6.69</v>
+      </c>
+      <c r="I831" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J831" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="832" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A832" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B832" s="2">
+        <v>13</v>
+      </c>
+      <c r="C832" s="2">
+        <v>85</v>
+      </c>
+      <c r="D832" s="2">
+        <v>3.2090000000000001</v>
+      </c>
+      <c r="E832" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="F832" s="2">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G832" s="2">
+        <f t="shared" si="474"/>
+        <v>5.65</v>
+      </c>
+      <c r="H832" s="2">
+        <f t="shared" si="473"/>
+        <v>6.8599999999999994</v>
+      </c>
+      <c r="I832" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J832" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="833" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A833" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B833" s="2">
+        <v>13</v>
+      </c>
+      <c r="C833" s="2">
+        <v>86</v>
+      </c>
+      <c r="D833" s="2">
+        <v>3.0179999999999998</v>
+      </c>
+      <c r="E833" s="2">
+        <v>56.7</v>
+      </c>
+      <c r="F833" s="2">
+        <v>68.7</v>
+      </c>
+      <c r="G833" s="2">
+        <f t="shared" si="474"/>
+        <v>5.67</v>
+      </c>
+      <c r="H833" s="2">
+        <f t="shared" si="473"/>
+        <v>6.87</v>
+      </c>
+      <c r="I833" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J833" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="834" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A834" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B834" s="2">
+        <v>13</v>
+      </c>
+      <c r="C834" s="2">
+        <v>87</v>
+      </c>
+      <c r="D834" s="2">
+        <v>3.9910000000000001</v>
+      </c>
+      <c r="E834" s="2">
+        <v>61</v>
+      </c>
+      <c r="F834" s="2">
+        <v>76.2</v>
+      </c>
+      <c r="G834" s="2">
+        <f t="shared" si="474"/>
+        <v>6.1</v>
+      </c>
+      <c r="H834" s="2">
+        <f t="shared" si="473"/>
+        <v>7.62</v>
+      </c>
+      <c r="I834" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J834" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="835" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A835" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B835" s="2">
+        <v>13</v>
+      </c>
+      <c r="C835" s="2">
+        <v>88</v>
+      </c>
+      <c r="D835" s="2">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="E835" s="2">
+        <v>59.9</v>
+      </c>
+      <c r="F835" s="2">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="G835" s="2">
+        <f t="shared" si="474"/>
+        <v>5.99</v>
+      </c>
+      <c r="H835" s="2">
+        <f t="shared" si="473"/>
+        <v>7.24</v>
+      </c>
+      <c r="I835" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J835" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="836" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A836" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B836" s="2">
+        <v>13</v>
+      </c>
+      <c r="C836" s="2">
+        <v>89</v>
+      </c>
+      <c r="D836" s="2">
+        <v>4.32</v>
+      </c>
+      <c r="E836" s="2">
+        <v>63.6</v>
+      </c>
+      <c r="F836" s="2">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="G836" s="2">
+        <f t="shared" si="474"/>
+        <v>6.36</v>
+      </c>
+      <c r="H836" s="2">
+        <f t="shared" si="473"/>
+        <v>7.69</v>
+      </c>
+      <c r="I836" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J836" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="837" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A837" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B837" s="2">
+        <v>13</v>
+      </c>
+      <c r="C837" s="2">
+        <v>90</v>
+      </c>
+      <c r="D837" s="2">
+        <v>5.6879999999999997</v>
+      </c>
+      <c r="E837" s="2">
+        <v>67.3</v>
+      </c>
+      <c r="F837" s="2">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="G837" s="2">
+        <f t="shared" si="474"/>
+        <v>6.7299999999999995</v>
+      </c>
+      <c r="H837" s="2">
+        <f t="shared" si="473"/>
+        <v>8.1900000000000013</v>
+      </c>
+      <c r="I837" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J837" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="838" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A838" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B838" s="2">
+        <v>13</v>
+      </c>
+      <c r="C838" s="2">
+        <v>91</v>
+      </c>
+      <c r="D838" s="2">
+        <v>4.9989999999999997</v>
+      </c>
+      <c r="E838" s="2">
+        <v>64.2</v>
+      </c>
+      <c r="F838" s="2">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="G838" s="2">
+        <f t="shared" si="474"/>
+        <v>6.42</v>
+      </c>
+      <c r="H838" s="2">
+        <f t="shared" si="473"/>
+        <v>7.94</v>
+      </c>
+      <c r="I838" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J838" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="839" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A839" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B839" s="2">
+        <v>13</v>
+      </c>
+      <c r="C839" s="2">
+        <v>92</v>
+      </c>
+      <c r="D839" s="2">
+        <v>4.3239999999999998</v>
+      </c>
+      <c r="E839" s="2">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F839" s="2">
+        <v>79.3</v>
+      </c>
+      <c r="G839" s="2">
+        <f t="shared" si="474"/>
+        <v>6.4599999999999991</v>
+      </c>
+      <c r="H839" s="2">
+        <f t="shared" si="473"/>
+        <v>7.93</v>
+      </c>
+      <c r="I839" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J839" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="840" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A840" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B840" s="2">
+        <v>13</v>
+      </c>
+      <c r="C840" s="2">
+        <v>93</v>
+      </c>
+      <c r="D840" s="2">
+        <v>5.0949999999999998</v>
+      </c>
+      <c r="E840" s="2">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="F840" s="2">
+        <v>80.8</v>
+      </c>
+      <c r="G840" s="2">
+        <f t="shared" si="474"/>
+        <v>6.6099999999999994</v>
+      </c>
+      <c r="H840" s="2">
+        <f t="shared" si="473"/>
+        <v>8.08</v>
+      </c>
+      <c r="I840" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J840" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="841" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A841" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B841" s="2">
+        <v>13</v>
+      </c>
+      <c r="C841" s="2">
+        <v>94</v>
+      </c>
+      <c r="D841" s="2">
+        <v>5.4189999999999996</v>
+      </c>
+      <c r="E841" s="2">
+        <v>68</v>
+      </c>
+      <c r="F841" s="2">
+        <v>82.9</v>
+      </c>
+      <c r="G841" s="2">
+        <f t="shared" si="474"/>
+        <v>6.8</v>
+      </c>
+      <c r="H841" s="2">
+        <f t="shared" si="473"/>
+        <v>8.2900000000000009</v>
+      </c>
+      <c r="I841" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J841" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="842" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A842" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B842" s="2">
+        <v>13</v>
+      </c>
+      <c r="C842" s="2">
+        <v>95</v>
+      </c>
+      <c r="D842" s="2">
+        <v>6.7249999999999996</v>
+      </c>
+      <c r="E842" s="2">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="F842" s="2">
+        <v>88.5</v>
+      </c>
+      <c r="G842" s="2">
+        <f t="shared" si="474"/>
+        <v>7.19</v>
+      </c>
+      <c r="H842" s="2">
+        <f t="shared" si="473"/>
+        <v>8.85</v>
+      </c>
+      <c r="I842" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J842" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="843" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A843" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B843" s="2">
+        <v>13</v>
+      </c>
+      <c r="C843" s="2">
+        <v>96</v>
+      </c>
+      <c r="D843" s="2">
+        <v>3.1920000000000002</v>
+      </c>
+      <c r="E843" s="2">
+        <v>56.4</v>
+      </c>
+      <c r="F843" s="2">
+        <v>70.5</v>
+      </c>
+      <c r="G843" s="2">
+        <f t="shared" si="474"/>
+        <v>5.64</v>
+      </c>
+      <c r="H843" s="2">
+        <f t="shared" si="473"/>
+        <v>7.05</v>
+      </c>
+      <c r="I843" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J843" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="844" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A844" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B844" s="2">
+        <v>13</v>
+      </c>
+      <c r="C844" s="2">
+        <v>97</v>
+      </c>
+      <c r="D844" s="2">
+        <v>1.069</v>
+      </c>
+      <c r="E844" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="F844" s="2">
+        <v>53.9</v>
+      </c>
+      <c r="G844" s="2">
+        <f t="shared" si="474"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="H844" s="2">
+        <f t="shared" si="473"/>
+        <v>5.39</v>
+      </c>
+      <c r="I844" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J844" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="845" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A845" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B845" s="2">
+        <v>13</v>
+      </c>
+      <c r="C845" s="2">
+        <v>98</v>
+      </c>
+      <c r="D845" s="2">
+        <v>6.266</v>
+      </c>
+      <c r="E845" s="2">
+        <v>73</v>
+      </c>
+      <c r="F845" s="2">
+        <v>87.6</v>
+      </c>
+      <c r="G845" s="2">
+        <f t="shared" si="474"/>
+        <v>7.3</v>
+      </c>
+      <c r="H845" s="2">
+        <f t="shared" si="473"/>
+        <v>8.76</v>
+      </c>
+      <c r="I845" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J845" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="846" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A846" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B846" s="2">
+        <v>13</v>
+      </c>
+      <c r="C846" s="2">
+        <v>99</v>
+      </c>
+      <c r="D846" s="2">
+        <v>4.7910000000000004</v>
+      </c>
+      <c r="E846" s="2">
+        <v>66.7</v>
+      </c>
+      <c r="F846" s="2">
+        <v>79.8</v>
+      </c>
+      <c r="G846" s="2">
+        <f t="shared" si="474"/>
+        <v>6.67</v>
+      </c>
+      <c r="H846" s="2">
+        <f t="shared" si="473"/>
+        <v>7.9799999999999995</v>
+      </c>
+      <c r="I846" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J846" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="847" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A847" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B847" s="2">
+        <v>13</v>
+      </c>
+      <c r="C847" s="2">
+        <v>100</v>
+      </c>
+      <c r="D847" s="2">
+        <v>4.3949999999999996</v>
+      </c>
+      <c r="E847" s="2">
+        <v>63.4</v>
+      </c>
+      <c r="F847" s="2">
+        <v>76</v>
+      </c>
+      <c r="G847" s="2">
+        <f t="shared" si="474"/>
+        <v>6.34</v>
+      </c>
+      <c r="H847" s="2">
+        <f t="shared" si="473"/>
+        <v>7.6</v>
+      </c>
+      <c r="I847" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J847" s="2">
+        <v>136804</v>
+      </c>
+    </row>
+    <row r="848" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A848" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B848" s="2">
+        <v>13</v>
+      </c>
+      <c r="C848" s="2">
+        <v>101</v>
+      </c>
+      <c r="D848" s="2">
+        <v>0.378</v>
+      </c>
+      <c r="E848" s="2">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="F848" s="2">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="G848" s="2">
+        <f t="shared" si="474"/>
+        <v>3.22</v>
+      </c>
+      <c r="H848" s="2">
+        <f t="shared" si="473"/>
+        <v>3.63</v>
+      </c>
+      <c r="I848" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J848" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="849" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A849" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B849" s="2">
+        <v>13</v>
+      </c>
+      <c r="C849" s="2">
+        <v>102</v>
+      </c>
+      <c r="D849" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="E849" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="F849" s="2">
+        <v>54.8</v>
+      </c>
+      <c r="G849" s="2">
+        <f t="shared" si="474"/>
+        <v>4.33</v>
+      </c>
+      <c r="H849" s="2">
+        <f t="shared" si="473"/>
+        <v>5.4799999999999995</v>
+      </c>
+      <c r="I849" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J849" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="850" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A850" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B850" s="2">
+        <v>13</v>
+      </c>
+      <c r="C850" s="2">
+        <v>103</v>
+      </c>
+      <c r="D850" s="2">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="E850" s="2">
+        <v>45.8</v>
+      </c>
+      <c r="F850" s="2">
+        <v>53.6</v>
+      </c>
+      <c r="G850" s="2">
+        <f t="shared" si="474"/>
+        <v>4.58</v>
+      </c>
+      <c r="H850" s="2">
+        <f t="shared" si="473"/>
+        <v>5.36</v>
+      </c>
+      <c r="I850" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J850" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="851" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A851" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B851" s="2">
+        <v>13</v>
+      </c>
+      <c r="C851" s="2">
+        <v>104</v>
+      </c>
+      <c r="D851" s="2">
+        <v>3.234</v>
+      </c>
+      <c r="E851" s="2">
+        <v>55.6</v>
+      </c>
+      <c r="F851" s="2">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="G851" s="2">
+        <f t="shared" si="474"/>
+        <v>5.5600000000000005</v>
+      </c>
+      <c r="H851" s="2">
+        <f t="shared" si="473"/>
+        <v>6.7099999999999991</v>
+      </c>
+      <c r="I851" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J851" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="852" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A852" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B852" s="2">
+        <v>13</v>
+      </c>
+      <c r="C852" s="2">
+        <v>105</v>
+      </c>
+      <c r="D852" s="2">
+        <v>1.1539999999999999</v>
+      </c>
+      <c r="E852" s="2">
+        <v>43.9</v>
+      </c>
+      <c r="F852" s="2">
+        <v>50.3</v>
+      </c>
+      <c r="G852" s="2">
+        <f t="shared" si="474"/>
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="H852" s="2">
+        <f t="shared" si="473"/>
+        <v>5.0299999999999994</v>
+      </c>
+      <c r="I852" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J852" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="853" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A853" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B853" s="2">
+        <v>13</v>
+      </c>
+      <c r="C853" s="2">
+        <v>106</v>
+      </c>
+      <c r="D853" s="2">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="E853" s="2">
+        <v>32</v>
+      </c>
+      <c r="F853" s="2">
+        <v>35.9</v>
+      </c>
+      <c r="G853" s="2">
+        <f t="shared" si="474"/>
+        <v>3.2</v>
+      </c>
+      <c r="H853" s="2">
+        <f t="shared" si="473"/>
+        <v>3.59</v>
+      </c>
+      <c r="I853" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J853" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="854" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A854" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B854" s="2">
+        <v>13</v>
+      </c>
+      <c r="C854" s="2">
+        <v>107</v>
+      </c>
+      <c r="D854" s="2">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E854" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="F854" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="G854" s="2">
+        <f t="shared" si="474"/>
+        <v>2.57</v>
+      </c>
+      <c r="H854" s="2">
+        <f t="shared" si="473"/>
+        <v>2.7199999999999998</v>
+      </c>
+      <c r="I854" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J854" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="855" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A855" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B855" s="2">
+        <v>13</v>
+      </c>
+      <c r="C855" s="2">
+        <v>108</v>
+      </c>
+      <c r="D855" s="2">
+        <v>0.159</v>
+      </c>
+      <c r="E855" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="F855" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="G855" s="2">
+        <f t="shared" si="474"/>
+        <v>2.4699999999999998</v>
+      </c>
+      <c r="H855" s="2">
+        <f t="shared" si="473"/>
+        <v>2.84</v>
+      </c>
+      <c r="I855" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J855" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="856" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A856" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B856" s="2">
+        <v>13</v>
+      </c>
+      <c r="C856" s="2">
+        <v>109</v>
+      </c>
+      <c r="D856" s="2">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E856" s="2">
+        <v>34.4</v>
+      </c>
+      <c r="F856" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="G856" s="2">
+        <f t="shared" si="474"/>
+        <v>3.44</v>
+      </c>
+      <c r="H856" s="2">
+        <f t="shared" si="473"/>
+        <v>4.07</v>
+      </c>
+      <c r="I856" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J856" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="857" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A857" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B857" s="2">
+        <v>13</v>
+      </c>
+      <c r="C857" s="2">
+        <v>110</v>
+      </c>
+      <c r="D857" s="2">
+        <v>1.2270000000000001</v>
+      </c>
+      <c r="E857" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="F857" s="2">
+        <v>49.5</v>
+      </c>
+      <c r="G857" s="2">
+        <f t="shared" si="474"/>
+        <v>4.33</v>
+      </c>
+      <c r="H857" s="2">
+        <f t="shared" si="473"/>
+        <v>4.95</v>
+      </c>
+      <c r="I857" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J857" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="858" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A858" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B858" s="2">
+        <v>13</v>
+      </c>
+      <c r="C858" s="2">
+        <v>111</v>
+      </c>
+      <c r="D858" s="2">
+        <v>2.1469999999999998</v>
+      </c>
+      <c r="E858" s="2">
+        <v>49.8</v>
+      </c>
+      <c r="F858" s="2">
+        <v>58.1</v>
+      </c>
+      <c r="G858" s="2">
+        <f t="shared" si="474"/>
+        <v>4.9799999999999995</v>
+      </c>
+      <c r="H858" s="2">
+        <f t="shared" si="473"/>
+        <v>5.8100000000000005</v>
+      </c>
+      <c r="I858" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J858" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="859" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A859" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B859" s="2">
+        <v>13</v>
+      </c>
+      <c r="C859" s="2">
+        <v>112</v>
+      </c>
+      <c r="D859" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="E859" s="2">
+        <v>27.1</v>
+      </c>
+      <c r="F859" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="G859" s="2">
+        <f t="shared" si="474"/>
+        <v>2.71</v>
+      </c>
+      <c r="H859" s="2">
+        <f t="shared" si="473"/>
+        <v>2.96</v>
+      </c>
+      <c r="I859" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J859" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="860" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A860" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B860" s="2">
+        <v>13</v>
+      </c>
+      <c r="C860" s="2">
+        <v>113</v>
+      </c>
+      <c r="D860" s="2">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E860" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="F860" s="2">
+        <v>29.1</v>
+      </c>
+      <c r="G860" s="2">
+        <f t="shared" si="474"/>
+        <v>2.75</v>
+      </c>
+      <c r="H860" s="2">
+        <f t="shared" si="473"/>
+        <v>2.91</v>
+      </c>
+      <c r="I860" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J860" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="861" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A861" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B861" s="2">
+        <v>13</v>
+      </c>
+      <c r="C861" s="2">
+        <v>114</v>
+      </c>
+      <c r="D861" s="2">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="E861" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="F861" s="2">
+        <v>48.6</v>
+      </c>
+      <c r="G861" s="2">
+        <f t="shared" si="474"/>
+        <v>4.05</v>
+      </c>
+      <c r="H861" s="2">
+        <f t="shared" si="473"/>
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="I861" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J861" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="862" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A862" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B862" s="2">
+        <v>13</v>
+      </c>
+      <c r="C862" s="2">
+        <v>115</v>
+      </c>
+      <c r="D862" s="2">
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="E862" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="F862" s="2">
+        <v>58.5</v>
+      </c>
+      <c r="G862" s="2">
+        <f t="shared" si="474"/>
+        <v>4.7700000000000005</v>
+      </c>
+      <c r="H862" s="2">
+        <f t="shared" si="473"/>
+        <v>5.85</v>
+      </c>
+      <c r="I862" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J862" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="863" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A863" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B863" s="2">
+        <v>13</v>
+      </c>
+      <c r="C863" s="2">
+        <v>116</v>
+      </c>
+      <c r="D863" s="2">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E863" s="2">
+        <v>30</v>
+      </c>
+      <c r="F863" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="G863" s="2">
+        <f t="shared" si="474"/>
+        <v>3</v>
+      </c>
+      <c r="H863" s="2">
+        <f t="shared" si="473"/>
+        <v>3.3899999999999997</v>
+      </c>
+      <c r="I863" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J863" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="864" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A864" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B864" s="2">
+        <v>13</v>
+      </c>
+      <c r="C864" s="2">
+        <v>117</v>
+      </c>
+      <c r="D864" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="E864" s="2">
+        <v>26.6</v>
+      </c>
+      <c r="F864" s="2">
+        <v>29.2</v>
+      </c>
+      <c r="G864" s="2">
+        <f t="shared" si="474"/>
+        <v>2.66</v>
+      </c>
+      <c r="H864" s="2">
+        <f t="shared" si="473"/>
+        <v>2.92</v>
+      </c>
+      <c r="I864" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J864" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="865" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A865" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B865" s="2">
+        <v>13</v>
+      </c>
+      <c r="C865" s="2">
+        <v>118</v>
+      </c>
+      <c r="D865" s="2">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="E865" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="F865" s="2">
+        <v>36.5</v>
+      </c>
+      <c r="G865" s="2">
+        <f t="shared" si="474"/>
+        <v>3.15</v>
+      </c>
+      <c r="H865" s="2">
+        <f t="shared" si="473"/>
+        <v>3.65</v>
+      </c>
+      <c r="I865" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J865" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="866" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A866" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B866" s="2">
+        <v>13</v>
+      </c>
+      <c r="C866" s="2">
+        <v>119</v>
+      </c>
+      <c r="D866" s="2">
+        <v>2.3069999999999999</v>
+      </c>
+      <c r="E866" s="2">
+        <v>48</v>
+      </c>
+      <c r="F866" s="2">
+        <v>57.2</v>
+      </c>
+      <c r="G866" s="2">
+        <f t="shared" si="474"/>
+        <v>4.8</v>
+      </c>
+      <c r="H866" s="2">
+        <f t="shared" si="473"/>
+        <v>5.7200000000000006</v>
+      </c>
+      <c r="I866" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J866" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="867" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A867" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B867" s="2">
+        <v>13</v>
+      </c>
+      <c r="C867" s="2">
+        <v>120</v>
+      </c>
+      <c r="D867" s="2">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E867" s="2">
+        <v>40.4</v>
+      </c>
+      <c r="F867" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="G867" s="2">
+        <f t="shared" si="474"/>
+        <v>4.04</v>
+      </c>
+      <c r="H867" s="2">
+        <f t="shared" si="473"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="I867" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J867" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="868" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A868" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B868" s="2">
+        <v>13</v>
+      </c>
+      <c r="C868" s="2">
+        <v>121</v>
+      </c>
+      <c r="D868" s="2">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E868" s="2">
+        <v>29.7</v>
+      </c>
+      <c r="F868" s="2">
+        <v>34.4</v>
+      </c>
+      <c r="G868" s="2">
+        <f t="shared" si="474"/>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="H868" s="2">
+        <f t="shared" si="473"/>
+        <v>3.44</v>
+      </c>
+      <c r="I868" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J868" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="869" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A869" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B869" s="2">
+        <v>13</v>
+      </c>
+      <c r="C869" s="2">
+        <v>122</v>
+      </c>
+      <c r="D869" s="2">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="E869" s="2">
+        <v>30.9</v>
+      </c>
+      <c r="F869" s="2">
+        <v>36.6</v>
+      </c>
+      <c r="G869" s="2">
+        <f t="shared" si="474"/>
+        <v>3.09</v>
+      </c>
+      <c r="H869" s="2">
+        <f t="shared" si="473"/>
+        <v>3.66</v>
+      </c>
+      <c r="I869" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J869" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="870" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A870" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B870" s="2">
+        <v>13</v>
+      </c>
+      <c r="C870" s="2">
+        <v>123</v>
+      </c>
+      <c r="D870" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E870" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="F870" s="2">
+        <v>28.7</v>
+      </c>
+      <c r="G870" s="2">
+        <f t="shared" si="474"/>
+        <v>2.57</v>
+      </c>
+      <c r="H870" s="2">
+        <f t="shared" si="473"/>
+        <v>2.87</v>
+      </c>
+      <c r="I870" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J870" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="871" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A871" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B871" s="2">
+        <v>13</v>
+      </c>
+      <c r="C871" s="2">
+        <v>124</v>
+      </c>
+      <c r="D871" s="2">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E871" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="F871" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="G871" s="2">
+        <f t="shared" si="474"/>
+        <v>2.3600000000000003</v>
+      </c>
+      <c r="H871" s="2">
+        <f t="shared" si="473"/>
+        <v>2.57</v>
+      </c>
+      <c r="I871" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J871" s="2">
+        <v>136818</v>
+      </c>
+    </row>
+    <row r="872" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A872" s="2"/>
+      <c r="B872" s="2"/>
+      <c r="C872" s="2"/>
+      <c r="D872" s="2"/>
+      <c r="I872" s="3"/>
+      <c r="J872" s="2"/>
+    </row>
+    <row r="873" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A873" s="2"/>
+      <c r="B873" s="2"/>
+      <c r="C873" s="2"/>
+      <c r="D873" s="2"/>
+      <c r="I873" s="3"/>
+      <c r="J873" s="2"/>
+    </row>
+    <row r="874" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A874" s="2"/>
+      <c r="B874" s="2"/>
+      <c r="C874" s="2"/>
+      <c r="D874" s="2"/>
+      <c r="I874" s="3"/>
+      <c r="J874" s="2"/>
+    </row>
+    <row r="875" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A875" s="2"/>
+      <c r="B875" s="2"/>
+      <c r="C875" s="2"/>
+      <c r="D875" s="2"/>
+      <c r="I875" s="3"/>
+      <c r="J875" s="2"/>
+    </row>
+    <row r="876" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A876" s="2"/>
+      <c r="B876" s="2"/>
+      <c r="C876" s="2"/>
+      <c r="D876" s="2"/>
+      <c r="I876" s="3"/>
+      <c r="J876" s="2"/>
+    </row>
+    <row r="877" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A877" s="2"/>
+      <c r="B877" s="2"/>
+      <c r="C877" s="2"/>
+      <c r="D877" s="2"/>
+      <c r="I877" s="3"/>
+      <c r="J877" s="2"/>
+    </row>
+    <row r="878" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A878" s="2"/>
+      <c r="B878" s="2"/>
+      <c r="C878" s="2"/>
+      <c r="D878" s="2"/>
+      <c r="I878" s="3"/>
+      <c r="J878" s="2"/>
+    </row>
+    <row r="879" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A879" s="2"/>
+      <c r="B879" s="2"/>
+      <c r="C879" s="2"/>
+      <c r="D879" s="2"/>
+      <c r="I879" s="3"/>
+      <c r="J879" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>